<commit_message>
this is the file I don't want...
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/EB_150326_A.xlsx
+++ b/Mouse_workbooks/EB_150326_A.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="738"/>
+    <workbookView xWindow="1180" yWindow="140" windowWidth="25600" windowHeight="16060" tabRatio="738" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Info" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -149,6 +149,45 @@
   </si>
   <si>
     <t>EB_150326_A</t>
+  </si>
+  <si>
+    <t>2015_04_17_0000</t>
+  </si>
+  <si>
+    <t>2015_04_17_0001</t>
+  </si>
+  <si>
+    <t>2015_04_17_0002</t>
+  </si>
+  <si>
+    <t>2015_04_17_0003</t>
+  </si>
+  <si>
+    <t>2015_04_17_0004</t>
+  </si>
+  <si>
+    <t>2015_04_17_0005</t>
+  </si>
+  <si>
+    <t>2015_04_17_0006</t>
+  </si>
+  <si>
+    <t>2015_04_17_0007</t>
+  </si>
+  <si>
+    <t>2015_04_17_0008</t>
+  </si>
+  <si>
+    <t>2015_04_17_0009</t>
+  </si>
+  <si>
+    <t>2015_04_17_0010</t>
+  </si>
+  <si>
+    <t>2015_04_17_0011</t>
+  </si>
+  <si>
+    <t>2015_04_17_0012</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1365,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:I7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0"/>
@@ -1476,8 +1515,12 @@
       <c r="I6" s="42"/>
     </row>
     <row r="7" spans="1:9" ht="39" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="36"/>
@@ -1487,8 +1530,12 @@
       <c r="I7" s="39"/>
     </row>
     <row r="8" spans="1:9" ht="39" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="36"/>
@@ -1498,8 +1545,12 @@
       <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:9" ht="39" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="36"/>
@@ -1509,8 +1560,12 @@
       <c r="I9" s="39"/>
     </row>
     <row r="10" spans="1:9" ht="39" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="36"/>
@@ -1520,8 +1575,12 @@
       <c r="I10" s="39"/>
     </row>
     <row r="11" spans="1:9" ht="39" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="36"/>
@@ -1531,8 +1590,12 @@
       <c r="I11" s="39"/>
     </row>
     <row r="12" spans="1:9" ht="39" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="36"/>
@@ -1542,8 +1605,12 @@
       <c r="I12" s="39"/>
     </row>
     <row r="13" spans="1:9" ht="39" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="36"/>
@@ -1553,8 +1620,12 @@
       <c r="I13" s="39"/>
     </row>
     <row r="14" spans="1:9" ht="39" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="36"/>
@@ -1564,8 +1635,12 @@
       <c r="I14" s="39"/>
     </row>
     <row r="15" spans="1:9" ht="39" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="36"/>
@@ -1575,8 +1650,12 @@
       <c r="I15" s="39"/>
     </row>
     <row r="16" spans="1:9" ht="39" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="36"/>
@@ -1586,8 +1665,12 @@
       <c r="I16" s="39"/>
     </row>
     <row r="17" spans="1:9" ht="39" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="36"/>
@@ -1597,8 +1680,12 @@
       <c r="I17" s="39"/>
     </row>
     <row r="18" spans="1:9" ht="39" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="36"/>
@@ -1608,8 +1695,12 @@
       <c r="I18" s="39"/>
     </row>
     <row r="19" spans="1:9" ht="39" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="36"/>
@@ -2622,7 +2713,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>